<commit_message>
update maven-compiler-plugin configuration in pom.xml
</commit_message>
<xml_diff>
--- a/target/classes/RequestParameters.xlsx
+++ b/target/classes/RequestParameters.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="regression" sheetId="1" r:id="rId1"/>
     <sheet name="stress" sheetId="2" r:id="rId2"/>
-    <sheet name="status" sheetId="3" r:id="rId3"/>
+    <sheet name="logCompare" sheetId="4" r:id="rId3"/>
+    <sheet name="status" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="39">
   <si>
     <t>scenario1</t>
   </si>
@@ -78,6 +79,66 @@
   </si>
   <si>
     <t>STRESS.bat</t>
+  </si>
+  <si>
+    <t>match</t>
+  </si>
+  <si>
+    <t>F41F42</t>
+  </si>
+  <si>
+    <t>comp</t>
+  </si>
+  <si>
+    <t>011GT000006</t>
+  </si>
+  <si>
+    <t>exclude</t>
+  </si>
+  <si>
+    <t>uatLog</t>
+  </si>
+  <si>
+    <t>C:\\FINsim\\UAT.mlg</t>
+  </si>
+  <si>
+    <t>productionLog</t>
+  </si>
+  <si>
+    <t>C:\\FINsim\\production.mlg</t>
+  </si>
+  <si>
+    <t>deviceName</t>
+  </si>
+  <si>
+    <t>device_name_1</t>
+  </si>
+  <si>
+    <t>reportName</t>
+  </si>
+  <si>
+    <t>reportName_1.rtf</t>
+  </si>
+  <si>
+    <t>location</t>
+  </si>
+  <si>
+    <t>C:\\FINsim\\</t>
+  </si>
+  <si>
+    <t>sprAddress</t>
+  </si>
+  <si>
+    <t>127.0.0.3</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>testValue</t>
+  </si>
+  <si>
+    <t>F43</t>
   </si>
 </sst>
 </file>
@@ -113,9 +174,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -530,8 +592,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -602,6 +664,169 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.140625" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" customWidth="1"/>
+    <col min="3" max="3" width="33.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="2">
+        <v>7011</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11">
+        <v>1721</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>

</xml_diff>

<commit_message>
debug status API in demo server
</commit_message>
<xml_diff>
--- a/target/classes/RequestParameters.xlsx
+++ b/target/classes/RequestParameters.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="regression" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="59">
   <si>
     <t>scenario1</t>
   </si>
@@ -151,12 +151,6 @@
   </si>
   <si>
     <t>C:\Users\abc.spr</t>
-  </si>
-  <si>
-    <t>RegRptFilePath</t>
-  </si>
-  <si>
-    <t>C:\Work\RegReport.rtf</t>
   </si>
   <si>
     <t>folderPath</t>
@@ -529,8 +523,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q7" sqref="Q7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -692,10 +686,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:C11"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -797,11 +791,11 @@
       <c r="A9" t="s">
         <v>11</v>
       </c>
-      <c r="B9" t="s">
-        <v>42</v>
-      </c>
-      <c r="C9" t="s">
-        <v>43</v>
+      <c r="B9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -809,20 +803,9 @@
         <v>11</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="1" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1045,10 +1028,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -1090,7 +1073,7 @@
         <v>34</v>
       </c>
       <c r="C2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1109,10 +1092,10 @@
         <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1120,7 +1103,7 @@
         <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C5">
         <v>1506081020</v>
@@ -1131,7 +1114,7 @@
         <v>0</v>
       </c>
       <c r="B6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C6">
         <v>1506093045</v>
@@ -1142,10 +1125,10 @@
         <v>0</v>
       </c>
       <c r="B7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -1153,10 +1136,10 @@
         <v>0</v>
       </c>
       <c r="B8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -1164,10 +1147,10 @@
         <v>0</v>
       </c>
       <c r="B9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -1175,10 +1158,10 @@
         <v>0</v>
       </c>
       <c r="B10" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -1190,7 +1173,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="T14" sqref="T14"/>
     </sheetView>
   </sheetViews>
@@ -1239,7 +1222,7 @@
         <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>13</v>
@@ -1253,7 +1236,7 @@
         <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>